<commit_message>
updated registration and AI to show on one page
</commit_message>
<xml_diff>
--- a/results/genetic_algorithm_results.xlsx
+++ b/results/genetic_algorithm_results.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F186"/>
+  <dimension ref="A1:F189"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4125,6 +4125,66 @@
         <v>3135</v>
       </c>
       <c r="F186">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>800</v>
+      </c>
+      <c r="B187">
+        <v>100</v>
+      </c>
+      <c r="C187">
+        <v>0.5</v>
+      </c>
+      <c r="D187">
+        <v>0.6</v>
+      </c>
+      <c r="E187">
+        <v>3397</v>
+      </c>
+      <c r="F187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>800</v>
+      </c>
+      <c r="B188">
+        <v>100</v>
+      </c>
+      <c r="C188">
+        <v>0.5</v>
+      </c>
+      <c r="D188">
+        <v>0.6</v>
+      </c>
+      <c r="E188">
+        <v>5887</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>800</v>
+      </c>
+      <c r="B189">
+        <v>100</v>
+      </c>
+      <c r="C189">
+        <v>0.5</v>
+      </c>
+      <c r="D189">
+        <v>0.6</v>
+      </c>
+      <c r="E189">
+        <v>11178</v>
+      </c>
+      <c r="F189">
         <v>-100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some tweaks before session
</commit_message>
<xml_diff>
--- a/results/genetic_algorithm_results.xlsx
+++ b/results/genetic_algorithm_results.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F228"/>
+  <dimension ref="A1:F234"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4965,6 +4965,126 @@
         <v>6911</v>
       </c>
       <c r="F228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>800</v>
+      </c>
+      <c r="B229">
+        <v>100</v>
+      </c>
+      <c r="C229">
+        <v>0.5</v>
+      </c>
+      <c r="D229">
+        <v>0.6</v>
+      </c>
+      <c r="E229">
+        <v>7123</v>
+      </c>
+      <c r="F229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>800</v>
+      </c>
+      <c r="B230">
+        <v>50</v>
+      </c>
+      <c r="C230">
+        <v>0.5</v>
+      </c>
+      <c r="D230">
+        <v>0.6</v>
+      </c>
+      <c r="E230">
+        <v>3395</v>
+      </c>
+      <c r="F230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>800</v>
+      </c>
+      <c r="B231">
+        <v>50</v>
+      </c>
+      <c r="C231">
+        <v>0.5</v>
+      </c>
+      <c r="D231">
+        <v>0.6</v>
+      </c>
+      <c r="E231">
+        <v>3409</v>
+      </c>
+      <c r="F231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>800</v>
+      </c>
+      <c r="B232">
+        <v>50</v>
+      </c>
+      <c r="C232">
+        <v>0.5</v>
+      </c>
+      <c r="D232">
+        <v>0.6</v>
+      </c>
+      <c r="E232">
+        <v>3344</v>
+      </c>
+      <c r="F232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>800</v>
+      </c>
+      <c r="B233">
+        <v>50</v>
+      </c>
+      <c r="C233">
+        <v>0.5</v>
+      </c>
+      <c r="D233">
+        <v>0.6</v>
+      </c>
+      <c r="E233">
+        <v>3089</v>
+      </c>
+      <c r="F233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>800</v>
+      </c>
+      <c r="B234">
+        <v>50</v>
+      </c>
+      <c r="C234">
+        <v>0.5</v>
+      </c>
+      <c r="D234">
+        <v>0.6</v>
+      </c>
+      <c r="E234">
+        <v>2107</v>
+      </c>
+      <c r="F234">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Editted ui colors and font
</commit_message>
<xml_diff>
--- a/results/genetic_algorithm_results.xlsx
+++ b/results/genetic_algorithm_results.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F235"/>
+  <dimension ref="A1:F240"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5105,6 +5105,106 @@
         <v>4932</v>
       </c>
       <c r="F235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>800</v>
+      </c>
+      <c r="B236">
+        <v>50</v>
+      </c>
+      <c r="C236">
+        <v>0.5</v>
+      </c>
+      <c r="D236">
+        <v>0.6</v>
+      </c>
+      <c r="E236">
+        <v>4584</v>
+      </c>
+      <c r="F236">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>800</v>
+      </c>
+      <c r="B237">
+        <v>50</v>
+      </c>
+      <c r="C237">
+        <v>0.5</v>
+      </c>
+      <c r="D237">
+        <v>0.6</v>
+      </c>
+      <c r="E237">
+        <v>2740</v>
+      </c>
+      <c r="F237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>800</v>
+      </c>
+      <c r="B238">
+        <v>50</v>
+      </c>
+      <c r="C238">
+        <v>0.5</v>
+      </c>
+      <c r="D238">
+        <v>0.6</v>
+      </c>
+      <c r="E238">
+        <v>2722</v>
+      </c>
+      <c r="F238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>800</v>
+      </c>
+      <c r="B239">
+        <v>50</v>
+      </c>
+      <c r="C239">
+        <v>0.5</v>
+      </c>
+      <c r="D239">
+        <v>0.6</v>
+      </c>
+      <c r="E239">
+        <v>4718</v>
+      </c>
+      <c r="F239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>800</v>
+      </c>
+      <c r="B240">
+        <v>50</v>
+      </c>
+      <c r="C240">
+        <v>0.5</v>
+      </c>
+      <c r="D240">
+        <v>0.6</v>
+      </c>
+      <c r="E240">
+        <v>4559</v>
+      </c>
+      <c r="F240">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
optimized AI and solved course offering problems
</commit_message>
<xml_diff>
--- a/results/genetic_algorithm_results.xlsx
+++ b/results/genetic_algorithm_results.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F252"/>
+  <dimension ref="A1:F300"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5445,6 +5445,966 @@
         <v>4930</v>
       </c>
       <c r="F252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>800</v>
+      </c>
+      <c r="B253">
+        <v>50</v>
+      </c>
+      <c r="C253">
+        <v>0.5</v>
+      </c>
+      <c r="D253">
+        <v>0.6</v>
+      </c>
+      <c r="E253">
+        <v>4648</v>
+      </c>
+      <c r="F253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>800</v>
+      </c>
+      <c r="B254">
+        <v>50</v>
+      </c>
+      <c r="C254">
+        <v>0.5</v>
+      </c>
+      <c r="D254">
+        <v>0.6</v>
+      </c>
+      <c r="E254">
+        <v>4569</v>
+      </c>
+      <c r="F254">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>800</v>
+      </c>
+      <c r="B255">
+        <v>50</v>
+      </c>
+      <c r="C255">
+        <v>0.5</v>
+      </c>
+      <c r="D255">
+        <v>0.6</v>
+      </c>
+      <c r="E255">
+        <v>2773</v>
+      </c>
+      <c r="F255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>800</v>
+      </c>
+      <c r="B256">
+        <v>50</v>
+      </c>
+      <c r="C256">
+        <v>0.5</v>
+      </c>
+      <c r="D256">
+        <v>0.6</v>
+      </c>
+      <c r="E256">
+        <v>4726</v>
+      </c>
+      <c r="F256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>800</v>
+      </c>
+      <c r="B257">
+        <v>50</v>
+      </c>
+      <c r="C257">
+        <v>0.5</v>
+      </c>
+      <c r="D257">
+        <v>0.6</v>
+      </c>
+      <c r="E257">
+        <v>5464</v>
+      </c>
+      <c r="F257">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>800</v>
+      </c>
+      <c r="B258">
+        <v>50</v>
+      </c>
+      <c r="C258">
+        <v>0.5</v>
+      </c>
+      <c r="D258">
+        <v>0.6</v>
+      </c>
+      <c r="E258">
+        <v>2784</v>
+      </c>
+      <c r="F258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>800</v>
+      </c>
+      <c r="B259">
+        <v>50</v>
+      </c>
+      <c r="C259">
+        <v>0.5</v>
+      </c>
+      <c r="D259">
+        <v>0.6</v>
+      </c>
+      <c r="E259">
+        <v>5126</v>
+      </c>
+      <c r="F259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>800</v>
+      </c>
+      <c r="B260">
+        <v>50</v>
+      </c>
+      <c r="C260">
+        <v>0.5</v>
+      </c>
+      <c r="D260">
+        <v>0.6</v>
+      </c>
+      <c r="E260">
+        <v>4583</v>
+      </c>
+      <c r="F260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>800</v>
+      </c>
+      <c r="B261">
+        <v>50</v>
+      </c>
+      <c r="C261">
+        <v>0.5</v>
+      </c>
+      <c r="D261">
+        <v>0.6</v>
+      </c>
+      <c r="E261">
+        <v>4590</v>
+      </c>
+      <c r="F261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>800</v>
+      </c>
+      <c r="B262">
+        <v>50</v>
+      </c>
+      <c r="C262">
+        <v>0.5</v>
+      </c>
+      <c r="D262">
+        <v>0.6</v>
+      </c>
+      <c r="E262">
+        <v>5144</v>
+      </c>
+      <c r="F262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>800</v>
+      </c>
+      <c r="B263">
+        <v>50</v>
+      </c>
+      <c r="C263">
+        <v>0.5</v>
+      </c>
+      <c r="D263">
+        <v>0.6</v>
+      </c>
+      <c r="E263">
+        <v>4397</v>
+      </c>
+      <c r="F263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>800</v>
+      </c>
+      <c r="B264">
+        <v>50</v>
+      </c>
+      <c r="C264">
+        <v>0.5</v>
+      </c>
+      <c r="D264">
+        <v>0.6</v>
+      </c>
+      <c r="E264">
+        <v>4757</v>
+      </c>
+      <c r="F264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>800</v>
+      </c>
+      <c r="B265">
+        <v>100</v>
+      </c>
+      <c r="C265">
+        <v>0.5</v>
+      </c>
+      <c r="D265">
+        <v>0.6</v>
+      </c>
+      <c r="E265">
+        <v>10327</v>
+      </c>
+      <c r="F265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>800</v>
+      </c>
+      <c r="B266">
+        <v>100</v>
+      </c>
+      <c r="C266">
+        <v>0.5</v>
+      </c>
+      <c r="D266">
+        <v>0.6</v>
+      </c>
+      <c r="E266">
+        <v>6517</v>
+      </c>
+      <c r="F266">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>800</v>
+      </c>
+      <c r="B267">
+        <v>100</v>
+      </c>
+      <c r="C267">
+        <v>0.5</v>
+      </c>
+      <c r="D267">
+        <v>0.7</v>
+      </c>
+      <c r="E267">
+        <v>12071</v>
+      </c>
+      <c r="F267">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>800</v>
+      </c>
+      <c r="B268">
+        <v>70</v>
+      </c>
+      <c r="C268">
+        <v>0.3</v>
+      </c>
+      <c r="D268">
+        <v>0.7</v>
+      </c>
+      <c r="E268">
+        <v>3338</v>
+      </c>
+      <c r="F268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>800</v>
+      </c>
+      <c r="B269">
+        <v>70</v>
+      </c>
+      <c r="C269">
+        <v>0.3</v>
+      </c>
+      <c r="D269">
+        <v>0.7</v>
+      </c>
+      <c r="E269">
+        <v>3236</v>
+      </c>
+      <c r="F269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>800</v>
+      </c>
+      <c r="B270">
+        <v>70</v>
+      </c>
+      <c r="C270">
+        <v>0.3</v>
+      </c>
+      <c r="D270">
+        <v>0.7</v>
+      </c>
+      <c r="E270">
+        <v>2806</v>
+      </c>
+      <c r="F270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>800</v>
+      </c>
+      <c r="B271">
+        <v>70</v>
+      </c>
+      <c r="C271">
+        <v>0.3</v>
+      </c>
+      <c r="D271">
+        <v>0.7</v>
+      </c>
+      <c r="E271">
+        <v>3941</v>
+      </c>
+      <c r="F271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>800</v>
+      </c>
+      <c r="B272">
+        <v>70</v>
+      </c>
+      <c r="C272">
+        <v>0.3</v>
+      </c>
+      <c r="D272">
+        <v>0.7</v>
+      </c>
+      <c r="E272">
+        <v>3820</v>
+      </c>
+      <c r="F272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>800</v>
+      </c>
+      <c r="B273">
+        <v>70</v>
+      </c>
+      <c r="C273">
+        <v>0.3</v>
+      </c>
+      <c r="D273">
+        <v>0.7</v>
+      </c>
+      <c r="E273">
+        <v>3734</v>
+      </c>
+      <c r="F273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>800</v>
+      </c>
+      <c r="B274">
+        <v>70</v>
+      </c>
+      <c r="C274">
+        <v>0.3</v>
+      </c>
+      <c r="D274">
+        <v>0.7</v>
+      </c>
+      <c r="E274">
+        <v>4230</v>
+      </c>
+      <c r="F274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>800</v>
+      </c>
+      <c r="B275">
+        <v>70</v>
+      </c>
+      <c r="C275">
+        <v>0.3</v>
+      </c>
+      <c r="D275">
+        <v>0.7</v>
+      </c>
+      <c r="E275">
+        <v>3706</v>
+      </c>
+      <c r="F275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>500</v>
+      </c>
+      <c r="B276">
+        <v>70</v>
+      </c>
+      <c r="C276">
+        <v>0.3</v>
+      </c>
+      <c r="D276">
+        <v>0.7</v>
+      </c>
+      <c r="E276">
+        <v>2683</v>
+      </c>
+      <c r="F276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>500</v>
+      </c>
+      <c r="B277">
+        <v>70</v>
+      </c>
+      <c r="C277">
+        <v>0.3</v>
+      </c>
+      <c r="D277">
+        <v>0.7</v>
+      </c>
+      <c r="E277">
+        <v>2699</v>
+      </c>
+      <c r="F277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>500</v>
+      </c>
+      <c r="B278">
+        <v>70</v>
+      </c>
+      <c r="C278">
+        <v>0.3</v>
+      </c>
+      <c r="D278">
+        <v>0.7</v>
+      </c>
+      <c r="E278">
+        <v>2430</v>
+      </c>
+      <c r="F278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>500</v>
+      </c>
+      <c r="B279">
+        <v>70</v>
+      </c>
+      <c r="C279">
+        <v>0.3</v>
+      </c>
+      <c r="D279">
+        <v>0.7</v>
+      </c>
+      <c r="E279">
+        <v>2765</v>
+      </c>
+      <c r="F279">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>500</v>
+      </c>
+      <c r="B280">
+        <v>70</v>
+      </c>
+      <c r="C280">
+        <v>0.3</v>
+      </c>
+      <c r="D280">
+        <v>0.7</v>
+      </c>
+      <c r="E280">
+        <v>1300</v>
+      </c>
+      <c r="F280">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>800</v>
+      </c>
+      <c r="B281">
+        <v>70</v>
+      </c>
+      <c r="C281">
+        <v>0.3</v>
+      </c>
+      <c r="D281">
+        <v>0.7</v>
+      </c>
+      <c r="E281">
+        <v>3609</v>
+      </c>
+      <c r="F281">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>800</v>
+      </c>
+      <c r="B282">
+        <v>70</v>
+      </c>
+      <c r="C282">
+        <v>0.6</v>
+      </c>
+      <c r="D282">
+        <v>0.7</v>
+      </c>
+      <c r="E282">
+        <v>4265</v>
+      </c>
+      <c r="F282">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>800</v>
+      </c>
+      <c r="B283">
+        <v>70</v>
+      </c>
+      <c r="C283">
+        <v>0.6</v>
+      </c>
+      <c r="D283">
+        <v>0.7</v>
+      </c>
+      <c r="E283">
+        <v>4130</v>
+      </c>
+      <c r="F283">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>800</v>
+      </c>
+      <c r="B284">
+        <v>70</v>
+      </c>
+      <c r="C284">
+        <v>0.6</v>
+      </c>
+      <c r="D284">
+        <v>0.7</v>
+      </c>
+      <c r="E284">
+        <v>4146</v>
+      </c>
+      <c r="F284">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>800</v>
+      </c>
+      <c r="B285">
+        <v>70</v>
+      </c>
+      <c r="C285">
+        <v>0.6</v>
+      </c>
+      <c r="D285">
+        <v>0.7</v>
+      </c>
+      <c r="E285">
+        <v>4342</v>
+      </c>
+      <c r="F285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>800</v>
+      </c>
+      <c r="B286">
+        <v>70</v>
+      </c>
+      <c r="C286">
+        <v>0.6</v>
+      </c>
+      <c r="D286">
+        <v>0.7</v>
+      </c>
+      <c r="E286">
+        <v>4278</v>
+      </c>
+      <c r="F286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>800</v>
+      </c>
+      <c r="B287">
+        <v>70</v>
+      </c>
+      <c r="C287">
+        <v>0.6</v>
+      </c>
+      <c r="D287">
+        <v>0.7</v>
+      </c>
+      <c r="E287">
+        <v>4156</v>
+      </c>
+      <c r="F287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>800</v>
+      </c>
+      <c r="B288">
+        <v>70</v>
+      </c>
+      <c r="C288">
+        <v>0.6</v>
+      </c>
+      <c r="D288">
+        <v>0.7</v>
+      </c>
+      <c r="E288">
+        <v>4154</v>
+      </c>
+      <c r="F288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>800</v>
+      </c>
+      <c r="B289">
+        <v>70</v>
+      </c>
+      <c r="C289">
+        <v>0.6</v>
+      </c>
+      <c r="D289">
+        <v>0.7</v>
+      </c>
+      <c r="E289">
+        <v>4293</v>
+      </c>
+      <c r="F289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>800</v>
+      </c>
+      <c r="B290">
+        <v>70</v>
+      </c>
+      <c r="C290">
+        <v>0.6</v>
+      </c>
+      <c r="D290">
+        <v>0.7</v>
+      </c>
+      <c r="E290">
+        <v>4325</v>
+      </c>
+      <c r="F290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>800</v>
+      </c>
+      <c r="B291">
+        <v>50</v>
+      </c>
+      <c r="C291">
+        <v>0.6</v>
+      </c>
+      <c r="D291">
+        <v>0.7</v>
+      </c>
+      <c r="E291">
+        <v>1289</v>
+      </c>
+      <c r="F291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>800</v>
+      </c>
+      <c r="B292">
+        <v>50</v>
+      </c>
+      <c r="C292">
+        <v>0.6</v>
+      </c>
+      <c r="D292">
+        <v>0.7</v>
+      </c>
+      <c r="E292">
+        <v>9238</v>
+      </c>
+      <c r="F292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>800</v>
+      </c>
+      <c r="B293">
+        <v>50</v>
+      </c>
+      <c r="C293">
+        <v>0.6</v>
+      </c>
+      <c r="D293">
+        <v>0.7</v>
+      </c>
+      <c r="E293">
+        <v>2603</v>
+      </c>
+      <c r="F293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>800</v>
+      </c>
+      <c r="B294">
+        <v>50</v>
+      </c>
+      <c r="C294">
+        <v>0.6</v>
+      </c>
+      <c r="D294">
+        <v>0.7</v>
+      </c>
+      <c r="E294">
+        <v>5298</v>
+      </c>
+      <c r="F294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>800</v>
+      </c>
+      <c r="B295">
+        <v>50</v>
+      </c>
+      <c r="C295">
+        <v>0.6</v>
+      </c>
+      <c r="D295">
+        <v>0.7</v>
+      </c>
+      <c r="E295">
+        <v>4145</v>
+      </c>
+      <c r="F295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>800</v>
+      </c>
+      <c r="B296">
+        <v>50</v>
+      </c>
+      <c r="C296">
+        <v>0.6</v>
+      </c>
+      <c r="D296">
+        <v>0.7</v>
+      </c>
+      <c r="E296">
+        <v>9047</v>
+      </c>
+      <c r="F296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>800</v>
+      </c>
+      <c r="B297">
+        <v>50</v>
+      </c>
+      <c r="C297">
+        <v>0.6</v>
+      </c>
+      <c r="D297">
+        <v>0.7</v>
+      </c>
+      <c r="E297">
+        <v>1366</v>
+      </c>
+      <c r="F297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>800</v>
+      </c>
+      <c r="B298">
+        <v>50</v>
+      </c>
+      <c r="C298">
+        <v>0.6</v>
+      </c>
+      <c r="D298">
+        <v>0.7</v>
+      </c>
+      <c r="E298">
+        <v>1372</v>
+      </c>
+      <c r="F298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>800</v>
+      </c>
+      <c r="B299">
+        <v>50</v>
+      </c>
+      <c r="C299">
+        <v>0.6</v>
+      </c>
+      <c r="D299">
+        <v>0.7</v>
+      </c>
+      <c r="E299">
+        <v>2134</v>
+      </c>
+      <c r="F299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>800</v>
+      </c>
+      <c r="B300">
+        <v>50</v>
+      </c>
+      <c r="C300">
+        <v>0.6</v>
+      </c>
+      <c r="D300">
+        <v>0.7</v>
+      </c>
+      <c r="E300">
+        <v>2105</v>
+      </c>
+      <c r="F300">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
small login form to avoid scrolling, removed unnecessary console.log, calculated gpa appear upon clicking btn
</commit_message>
<xml_diff>
--- a/results/genetic_algorithm_results.xlsx
+++ b/results/genetic_algorithm_results.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F300"/>
+  <dimension ref="A1:F304"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6405,6 +6405,86 @@
         <v>2105</v>
       </c>
       <c r="F300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>800</v>
+      </c>
+      <c r="B301">
+        <v>50</v>
+      </c>
+      <c r="C301">
+        <v>0.6</v>
+      </c>
+      <c r="D301">
+        <v>0.7</v>
+      </c>
+      <c r="E301">
+        <v>3432</v>
+      </c>
+      <c r="F301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>800</v>
+      </c>
+      <c r="B302">
+        <v>50</v>
+      </c>
+      <c r="C302">
+        <v>0.6</v>
+      </c>
+      <c r="D302">
+        <v>0.7</v>
+      </c>
+      <c r="E302">
+        <v>2551</v>
+      </c>
+      <c r="F302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>800</v>
+      </c>
+      <c r="B303">
+        <v>50</v>
+      </c>
+      <c r="C303">
+        <v>0.6</v>
+      </c>
+      <c r="D303">
+        <v>0.7</v>
+      </c>
+      <c r="E303">
+        <v>3411</v>
+      </c>
+      <c r="F303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>800</v>
+      </c>
+      <c r="B304">
+        <v>50</v>
+      </c>
+      <c r="C304">
+        <v>0.6</v>
+      </c>
+      <c r="D304">
+        <v>0.7</v>
+      </c>
+      <c r="E304">
+        <v>3997</v>
+      </c>
+      <c r="F304">
         <v>0</v>
       </c>
     </row>

</xml_diff>